<commit_message>
Add EVE side data
</commit_message>
<xml_diff>
--- a/tabular/eve/efv-side-data.xlsx
+++ b/tabular/eve/efv-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flaviviridae-GLUE/tabular/eve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/RNA/Flavivirus-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4CAC47-90ED-9E4F-A73E-9DB5ADD79B2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F002580-ACB4-5D41-9BB1-DA2A9E206342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6880" yWindow="640" windowWidth="37480" windowHeight="28160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6880" yWindow="500" windowWidth="37480" windowHeight="27040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -4895,8 +4895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
-      <selection activeCell="A317" sqref="A317"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>